<commit_message>
v2_lang_qmd - made sure the ODE kable has 11 years of data, made ggplot stacked bar for exit reasons by languages
</commit_message>
<xml_diff>
--- a/Data/ODE 13_18.xlsx
+++ b/Data/ODE 13_18.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF0D6827-4E99-3D4D-8055-D1E4861D6F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A36FA25-F0C6-CD4C-939C-28BA31495EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="15940" xr2:uid="{02BA0CDD-88FE-421E-A9B1-DFCA4A0669F1}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="19800" windowHeight="12900" xr2:uid="{02BA0CDD-88FE-421E-A9B1-DFCA4A0669F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data 2013-14 to 2017-18" sheetId="4" r:id="rId1"/>
     <sheet name="Data 2018-19 to 2022-23" sheetId="1" r:id="rId2"/>
     <sheet name="Primary Language" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3298998B-028A-458F-84C9-28908A90266A}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>